<commit_message>
Updated dataset code; re-trained neural nets; Fixed ground truth for mode; completed lime analysis
</commit_message>
<xml_diff>
--- a/data/lime-analysis.xlsx
+++ b/data/lime-analysis.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\archg\school\senoir\xai-senior-design\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3F7597C3-161E-4924-9ABE-F100A359F86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{715B339A-4F4B-4F15-929E-8C7B0E59F587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="2115" windowWidth="15885" windowHeight="14025"/>
+    <workbookView xWindow="960" yWindow="1740" windowWidth="17880" windowHeight="18945"/>
   </bookViews>
   <sheets>
-    <sheet name="lime-avg1_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Analysis" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>mode</t>
   </si>
@@ -37,33 +37,6 @@
     <t>tf</t>
   </si>
   <si>
-    <t>Lime</t>
-  </si>
-  <si>
-    <t>GT</t>
-  </si>
-  <si>
-    <t>1_1</t>
-  </si>
-  <si>
-    <t>avg</t>
-  </si>
-  <si>
-    <t>var</t>
-  </si>
-  <si>
-    <t>stdev</t>
-  </si>
-  <si>
-    <t>std</t>
-  </si>
-  <si>
-    <t>1_2</t>
-  </si>
-  <si>
-    <t>2_1</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
@@ -71,6 +44,42 @@
   </si>
   <si>
     <t>tt</t>
+  </si>
+  <si>
+    <t>Dataset 1, Model 1; Model Accuracy 79.91%</t>
+  </si>
+  <si>
+    <t>Dataset 1, Model 2; Model Accuracy 65.45%</t>
+  </si>
+  <si>
+    <t>Lime Avg</t>
+  </si>
+  <si>
+    <t>GT Avg</t>
+  </si>
+  <si>
+    <t>Diff STD</t>
+  </si>
+  <si>
+    <t>Lime STD</t>
+  </si>
+  <si>
+    <t>Diff Avg</t>
+  </si>
+  <si>
+    <t>GT STD</t>
+  </si>
+  <si>
+    <t>Dataset 2, Model 1; Model Accuracy 96.35%</t>
+  </si>
+  <si>
+    <t>DS1 Lime Diff</t>
+  </si>
+  <si>
+    <t>DS2 Lime Diff</t>
+  </si>
+  <si>
+    <t>Dataset 2, Model 2; Model Accuracy 92.50%</t>
   </si>
 </sst>
 </file>
@@ -554,12 +563,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -915,543 +925,641 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>1.1342712335534601E-5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.0116676725005001E-6</v>
+      <c r="B3">
+        <v>-2.0495981353685799E-2</v>
+      </c>
+      <c r="C3">
+        <v>2.9738483202574901E-2</v>
       </c>
       <c r="D3">
-        <f>_xlfn.VAR.P(B3:C3)</f>
-        <v>2.1767098625884292E-11</v>
+        <v>-5.0234464556260697E-2</v>
       </c>
       <c r="E3">
-        <f>SQRT(D3)</f>
-        <v>4.6655223315170504E-6</v>
-      </c>
-      <c r="G3" s="1">
-        <v>-4.0130942666747497E-6</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2.0068231988761701E-6</v>
-      </c>
-      <c r="I3">
-        <f>_xlfn.VAR.P(G3:H3)</f>
-        <v>9.059851573011254E-12</v>
+        <v>0.117298051746538</v>
+      </c>
+      <c r="F3">
+        <v>1.9998290151026998E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.12264425996690601</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
       </c>
       <c r="J3">
-        <f>SQRT(I3)</f>
-        <v>3.0099587327754601E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.4068181542356701E-3</v>
+      </c>
+      <c r="K3">
+        <v>2.3809523809523801E-2</v>
+      </c>
+      <c r="L3">
+        <v>-2.0402705655288102E-2</v>
+      </c>
+      <c r="M3">
+        <v>6.6592649104829801E-2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3.46944695195361E-18</v>
+      </c>
+      <c r="O3">
+        <v>6.6592649104829801E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>-1.9124312622255399E-5</v>
+      <c r="B4">
+        <v>4.5191319810269699E-2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3.9436733051699799E-2</v>
       </c>
       <c r="D4">
-        <f>_xlfn.VAR.P(B4:C4)</f>
-        <v>9.14348333184393E-11</v>
+        <v>5.7545867585699099E-3</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E7" si="0">SQRT(D4)</f>
-        <v>9.5621563111276997E-6</v>
-      </c>
-      <c r="G4" s="1">
-        <v>-8.8851073957017902E-6</v>
-      </c>
-      <c r="H4" s="1">
-        <v>6.0204695966285302E-6</v>
-      </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I7" si="1">_xlfn.VAR.P(G4:H4)</f>
-        <v>5.5544056368571749E-11</v>
+        <v>9.1575492115743298E-2</v>
+      </c>
+      <c r="F4">
+        <v>2.5765382378255399E-2</v>
+      </c>
+      <c r="G4">
+        <v>9.7552749134230898E-2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J7" si="2">SQRT(I4)</f>
-        <v>7.4527884961651602E-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.17652983085722701</v>
+      </c>
+      <c r="K4">
+        <v>7.43150183150183E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.102214812542209</v>
+      </c>
+      <c r="M4">
+        <v>0.27522779168114703</v>
+      </c>
+      <c r="N4">
+        <v>4.60212433162384E-2</v>
+      </c>
+      <c r="O4">
+        <v>0.242015055821758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>1.2324479135449301E-5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4.0233353450010002E-6</v>
+      <c r="B5">
+        <v>5.8427120641542103E-2</v>
+      </c>
+      <c r="C5">
+        <v>3.3582780124723398E-2</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D4:D7" si="3">_xlfn.VAR.P(B5:C5)</f>
-        <v>1.7227247057424593E-11</v>
+        <v>2.4844340516818698E-2</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>4.1505718952241502E-6</v>
+        <v>0.17869430132866801</v>
+      </c>
+      <c r="F5">
+        <v>1.44537128142777E-2</v>
       </c>
       <c r="G5">
-        <v>1.51121644546374E-4</v>
-      </c>
-      <c r="H5" s="1">
-        <v>8.0272927955047093E-6</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>5.118998375750377E-9</v>
+        <v>0.17434716034254899</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>7.1547175875434643E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.70329936670425E-2</v>
+      </c>
+      <c r="K5">
+        <v>5.5384615384615303E-2</v>
+      </c>
+      <c r="L5">
+        <v>-8.3516217175728102E-3</v>
+      </c>
+      <c r="M5">
+        <v>0.14382761322186299</v>
+      </c>
+      <c r="N5">
+        <v>1.7815508271580401E-2</v>
+      </c>
+      <c r="O5">
+        <v>0.1377189759621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <v>-1.11232968066955E-5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4.2245021122510504E-6</v>
+      <c r="B6">
+        <v>2.59203478923846E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.7024325704470501E-2</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
-        <v>5.8888732914104223E-11</v>
+        <v>-1.1039778120858601E-3</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>7.6738994594732748E-6</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3.9079263744870004E-6</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5.2794887231973298E-6</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>4.7029581909994883E-13</v>
+        <v>0.101543782178773</v>
+      </c>
+      <c r="F6">
+        <v>8.0924129408449508E-3</v>
+      </c>
+      <c r="G6">
+        <v>9.3542818170530506E-2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>6.8578117435516469E-7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.177939445988539</v>
+      </c>
+      <c r="K6">
+        <v>7.0480034188034196E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.107459411800504</v>
+      </c>
+      <c r="M6">
+        <v>0.307441951646093</v>
+      </c>
+      <c r="N6">
+        <v>4.54530941086548E-2</v>
+      </c>
+      <c r="O6">
+        <v>0.27724792337823501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
-        <v>5.3728182362907399E-5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.50875075437537E-5</v>
+      <c r="B7">
+        <v>5.0740220101788198E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.9809897404948703E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
-        <v>3.7327543761989463E-10</v>
+        <v>1.09303226968395E-2</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1.9320337409576849E-5</v>
-      </c>
-      <c r="G7" s="1">
-        <v>-2.6347936804987899E-6</v>
-      </c>
-      <c r="H7" s="1">
-        <v>3.01023479831426E-6</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>7.966586631652596E-12</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>2.8225142394065252E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <f>AVERAGE(B3:B7)</f>
-        <v>9.4295528809880797E-6</v>
-      </c>
-      <c r="C9" s="1">
-        <f>AVERAGE(C3:C7)</f>
-        <v>5.0694025347012503E-6</v>
-      </c>
-      <c r="D9" s="1">
-        <f>AVERAGE(D3:D7)</f>
-        <v>1.125186699071494E-10</v>
-      </c>
-      <c r="E9" s="1">
-        <f>AVERAGE(E3:E7)</f>
-        <v>9.0744974813838039E-6</v>
-      </c>
-      <c r="G9" s="1">
-        <f>AVERAGE(G3:G7)</f>
-        <v>2.7899315115597138E-5</v>
-      </c>
-      <c r="H9" s="1">
-        <f>AVERAGE(H3:H7)</f>
-        <v>4.8688618225042005E-6</v>
-      </c>
-      <c r="I9" s="1">
-        <f t="shared" ref="I9:J9" si="4">AVERAGE(I3:I7)</f>
-        <v>1.0384078332285426E-9</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="4"/>
-        <v>1.7103643703627394E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>9.4798616532149896E-2</v>
+      </c>
+      <c r="F7">
+        <v>2.23066148032511E-2</v>
+      </c>
+      <c r="G7">
+        <v>7.7436487050668606E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <f>_xlfn.VAR.P(B9:C9)</f>
-        <v>4.7527277605562891E-12</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="G10" s="2">
-        <f>_xlfn.VAR.P(G9:H9)</f>
-        <v>1.3260044472133382E-10</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="1"/>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>2.3416142488792602E-3</v>
+      </c>
+      <c r="K10">
+        <v>2.3809523809523801E-2</v>
+      </c>
+      <c r="L10">
+        <v>-2.14679095606445E-2</v>
+      </c>
+      <c r="M10">
+        <v>6.1294420269599102E-2</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>6.1294420269599102E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <f>SQRT(B10)</f>
-        <v>2.1800751731434147E-6</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="G11" s="2">
-        <f>SQRT(G10)</f>
-        <v>1.1515226646546468E-5</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1.83437166761346E-3</v>
+      </c>
+      <c r="C11">
+        <v>2.9626730885009001E-2</v>
+      </c>
+      <c r="D11">
+        <f>B11-C11</f>
+        <v>-2.7792359217395542E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.117725833055862</v>
+      </c>
+      <c r="F11">
+        <v>1.99965164508169E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.11978742609102599</v>
+      </c>
+      <c r="I11" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="J11">
+        <v>0.207395952547937</v>
+      </c>
+      <c r="K11">
+        <v>7.4067558057705804E-2</v>
+      </c>
+      <c r="L11">
+        <v>0.13332839449023101</v>
+      </c>
+      <c r="M11">
+        <v>0.32324249703116698</v>
+      </c>
+      <c r="N11">
+        <v>4.5671003690805199E-2</v>
+      </c>
+      <c r="O11">
+        <v>0.28956224645338402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>5.01327596776125E-2</v>
+      </c>
+      <c r="C12">
+        <v>3.9209311659642698E-2</v>
+      </c>
+      <c r="D12">
+        <f>B12-C12</f>
+        <v>1.0923448017969802E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.102928370139118</v>
+      </c>
+      <c r="F12">
+        <v>2.5525520858920799E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.114006315123322</v>
+      </c>
+      <c r="I12" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>3.9683041028201797E-2</v>
+      </c>
+      <c r="K12">
+        <v>5.4754085542262798E-2</v>
+      </c>
+      <c r="L12">
+        <v>-1.5071044514061001E-2</v>
+      </c>
+      <c r="M12">
+        <v>0.11897299445619</v>
+      </c>
+      <c r="N12">
+        <v>1.8090132615934399E-2</v>
+      </c>
+      <c r="O12">
+        <v>0.113635551043821</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>4.2739635309780102E-2</v>
+      </c>
+      <c r="C13">
+        <v>3.2769416014449097E-2</v>
+      </c>
+      <c r="D13">
+        <f>B13-C13</f>
+        <v>9.9702192953310051E-3</v>
+      </c>
+      <c r="E13">
+        <v>0.18428721874738599</v>
+      </c>
+      <c r="F13">
+        <v>1.33567579127089E-2</v>
+      </c>
+      <c r="G13">
+        <v>0.18067127044888601</v>
+      </c>
+      <c r="I13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>0.118912807928578</v>
+      </c>
+      <c r="K13">
+        <v>6.9678617855188002E-2</v>
+      </c>
+      <c r="L13">
+        <v>4.9234190073390902E-2</v>
+      </c>
+      <c r="M13">
+        <v>0.26601337178513002</v>
+      </c>
+      <c r="N13">
+        <v>4.6407819093776198E-2</v>
+      </c>
+      <c r="O13">
+        <v>0.24339998980289501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>1.6993855596726799E-2</v>
+      </c>
+      <c r="C14">
+        <v>2.6982617823677401E-2</v>
+      </c>
+      <c r="D14">
+        <f>B14-C14</f>
+        <v>-9.9887622269506024E-3</v>
+      </c>
+      <c r="E14">
+        <v>6.96715857827922E-2</v>
+      </c>
+      <c r="F14">
+        <v>7.8609481318396394E-3</v>
+      </c>
+      <c r="G14">
+        <v>6.2504757199360397E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.9513350758482301E-7</v>
-      </c>
-      <c r="C15" s="1">
-        <v>9.7680097680097605E-6</v>
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>5.0569382672862498E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.3939393939393903E-2</v>
       </c>
       <c r="D15">
-        <f>_xlfn.VAR.P(B15:C15)</f>
-        <v>2.2909989974351836E-11</v>
+        <f>B15-C15</f>
+        <v>6.6299887334685947E-3</v>
       </c>
       <c r="E15">
-        <f>SQRT(D15)</f>
-        <v>4.7864381302124685E-6</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3.1748947162806798E-6</v>
-      </c>
-      <c r="H15" s="1">
-        <v>9.7740245523496705E-6</v>
-      </c>
-      <c r="I15">
-        <f>_xlfn.VAR.P(G15:H15)</f>
-        <v>1.0887128648323986E-11</v>
-      </c>
-      <c r="J15">
-        <f>SQRT(I15)</f>
-        <v>3.2995649180344951E-6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>1.6993866844921301E-4</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2.9304029304029299E-5</v>
-      </c>
-      <c r="D16">
-        <f t="shared" ref="D16:D18" si="5">_xlfn.VAR.P(B16:C16)</f>
-        <v>4.9445254318740101E-9</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ref="E16:E18" si="6">SQRT(D16)</f>
-        <v>7.0317319572591857E-5</v>
-      </c>
-      <c r="G16" s="1">
-        <v>4.3100385622198298E-6</v>
-      </c>
-      <c r="H16" s="1">
-        <v>9.7740245523496705E-6</v>
-      </c>
-      <c r="I16">
-        <f t="shared" ref="I16:I18" si="7">_xlfn.VAR.P(G16:H16)</f>
-        <v>7.4637857250837936E-12</v>
-      </c>
-      <c r="J16">
-        <f t="shared" ref="J16:J18" si="8">SQRT(I16)</f>
-        <v>2.7319929950649204E-6</v>
-      </c>
+        <v>9.61001472198761E-2</v>
+      </c>
+      <c r="F15">
+        <v>2.1921629411073899E-2</v>
+      </c>
+      <c r="G15">
+        <v>8.3013970461169595E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1">
-        <v>-2.4174542033521898E-9</v>
-      </c>
-      <c r="C17" s="1">
-        <v>9.7680097680097605E-6</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="5"/>
-        <v>2.3865312026140761E-11</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="6"/>
-        <v>4.8852136111065565E-6</v>
-      </c>
-      <c r="G17" s="1">
-        <v>-5.2464152873252E-6</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1.4661036828524501E-5</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="7"/>
-        <v>9.9076662436212178E-11</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="8"/>
-        <v>9.9537260579248499E-6</v>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="J17" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1">
-        <v>8.5057191363121898E-6</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1.0083028083028001E-5</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="5"/>
-        <v>6.2197587834743513E-13</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="6"/>
-        <v>7.8865447335790539E-7</v>
-      </c>
-      <c r="G18">
-        <v>1.69423311141848E-4</v>
-      </c>
-      <c r="H18" s="1">
-        <v>2.68785675189616E-5</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="7"/>
-        <v>5.0797509836286025E-9</v>
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <f>B3-B11</f>
+        <v>-2.2330353021299258E-2</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" t="s">
+        <v>0</v>
       </c>
       <c r="J18">
-        <f t="shared" si="8"/>
-        <v>7.1272371811443197E-5</v>
+        <f>J3-J10</f>
+        <v>1.0652039053564099E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <f>B4-B12</f>
+        <v>-4.9414398673428006E-3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ref="J19:J21" si="0">J4-J11</f>
+        <v>-3.0866121690709986E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="1">
-        <f>AVERAGE(B15:B18)</f>
-        <v>4.4659275909726673E-5</v>
-      </c>
-      <c r="C20" s="1">
-        <f>AVERAGE(C15:C18)</f>
-        <v>1.4730769230769203E-5</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" ref="D20:E20" si="9">AVERAGE(D15:D18)</f>
-        <v>1.2479806774382125E-9</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="9"/>
-        <v>2.0194406446817195E-5</v>
-      </c>
-      <c r="G20" s="1">
-        <f>AVERAGE(G15:G18)</f>
-        <v>4.2915457283255829E-5</v>
-      </c>
-      <c r="H20" s="1">
-        <f>AVERAGE(H15:H18)</f>
-        <v>1.5271913363046362E-5</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" ref="I20:J20" si="10">AVERAGE(I15:I18)</f>
-        <v>1.2992946401095557E-9</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="10"/>
-        <v>2.1814413945616864E-5</v>
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B19:B22" si="1">B5-B13</f>
+        <v>1.5687485331762001E-2</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>7.3499526388407024E-3</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2">
-        <f>_xlfn.VAR.P(B20:C20)</f>
-        <v>2.2392887800810046E-10</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="G21" s="2">
-        <f>_xlfn.VAR.P(G20:H20)</f>
-        <v>1.9104138011713745E-10</v>
-      </c>
-      <c r="H21" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>8.9264922956578015E-3</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>5.9026638059961001E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="2">
-        <f>SQRT(B21)</f>
-        <v>1.4964253339478735E-5</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="G22" s="2">
-        <f>SQRT(G21)</f>
-        <v>1.3821771960104733E-5</v>
-      </c>
-      <c r="H22" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>1.7083742892570059E-4</v>
+      </c>
+      <c r="H22" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
+  <mergeCells count="4">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>